<commit_message>
update Signed-off-by: YooSeongHyun <wtnghw@naver.com>
</commit_message>
<xml_diff>
--- a/shyoo_20150920.xlsx
+++ b/shyoo_20150920.xlsx
@@ -8427,7 +8427,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>531</v>
       </c>
@@ -10584,7 +10584,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
etetet Signed-off-by: YooSeongHyun <wtnghw@naver.com>
</commit_message>
<xml_diff>
--- a/shyoo_20150920.xlsx
+++ b/shyoo_20150920.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19380" windowHeight="7980" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19380" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="진행률" sheetId="5" r:id="rId1"/>
@@ -4684,184 +4684,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>297077</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="사각형 설명선 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1933575" y="2219325"/>
-          <a:ext cx="1573427" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -29913"/>
-            <a:gd name="adj2" fmla="val -484351"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:srgbClr val="ED7D31">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:srgbClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:srgbClr val="ED7D31">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:srgbClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:srgbClr val="ED7D31">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:srgbClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="ED7D31"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
-          <a:prstTxWarp prst="textNoShape">
-            <a:avLst/>
-          </a:prstTxWarp>
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="ko-KR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="맑은 고딕" panose="020F0502020204030204"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="맑은 고딕" panose="020F0502020204030204"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="맑은 고딕" panose="020F0502020204030204"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="맑은 고딕" panose="020F0502020204030204"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="맑은 고딕" panose="020F0502020204030204"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="맑은 고딕" panose="020F0502020204030204"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="맑은 고딕" panose="020F0502020204030204"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="맑은 고딕" panose="020F0502020204030204"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="1" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="맑은 고딕" panose="020F0502020204030204"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="ko-KR" altLang="en-US" sz="1000"/>
-            <a:t>개수다름</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -5151,8 +4973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5354,7 +5176,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8576,7 +8397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D163" sqref="D163"/>
     </sheetView>
@@ -12198,8 +12019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>